<commit_message>
Update runner's complexity counter and visualizer's reduction calculation logics
</commit_message>
<xml_diff>
--- a/experiment_results/manual_vs_auto.xlsx
+++ b/experiment_results/manual_vs_auto.xlsx
@@ -493,7 +493,7 @@
         <v>170</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0</v>
@@ -533,7 +533,7 @@
         <v>146</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>0</v>
@@ -577,7 +577,7 @@
         <v>290</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>5</v>
@@ -597,7 +597,7 @@
         <v>571</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>7</v>
@@ -617,7 +617,7 @@
         <v>421</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>17</v>
@@ -637,7 +637,7 @@
         <v>647</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>12</v>
@@ -661,7 +661,7 @@
         <v>753</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>17</v>
@@ -681,7 +681,7 @@
         <v>940</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>7.5</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>17</v>
@@ -701,7 +701,7 @@
         <v>805</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>18</v>
@@ -721,7 +721,7 @@
         <v>992</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>18</v>
@@ -745,7 +745,7 @@
         <v>276</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>6</v>
@@ -765,7 +765,7 @@
         <v>423</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F15" s="3" t="n">
         <v>6</v>
@@ -785,7 +785,7 @@
         <v>339</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>8</v>
@@ -805,7 +805,7 @@
         <v>475</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F17" s="3" t="n">
         <v>8</v>
@@ -829,7 +829,7 @@
         <v>541</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>7</v>
@@ -849,7 +849,7 @@
         <v>650</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F19" s="3" t="n">
         <v>6</v>
@@ -869,7 +869,7 @@
         <v>897</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>18</v>
@@ -889,7 +889,7 @@
         <v>1019</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>17</v>
@@ -913,7 +913,7 @@
         <v>643</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F22" s="3" t="n">
         <v>13</v>
@@ -933,7 +933,7 @@
         <v>741</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F23" s="3" t="n">
         <v>12</v>
@@ -953,7 +953,7 @@
         <v>1422</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F24" s="3" t="n">
         <v>23</v>
@@ -973,7 +973,7 @@
         <v>1502</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F25" s="3" t="n">
         <v>22</v>
@@ -997,7 +997,7 @@
         <v>798</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="F26" s="3" t="n">
         <v>18</v>
@@ -1017,7 +1017,7 @@
         <v>939</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="F27" s="3" t="n">
         <v>17</v>
@@ -1037,7 +1037,7 @@
         <v>824</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F28" s="3" t="n">
         <v>19</v>
@@ -1057,7 +1057,7 @@
         <v>965</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F29" s="3" t="n">
         <v>18</v>
@@ -1081,7 +1081,7 @@
         <v>421</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F30" s="3" t="n">
         <v>5</v>
@@ -1101,7 +1101,7 @@
         <v>534</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F31" s="3" t="n">
         <v>5</v>
@@ -1121,7 +1121,7 @@
         <v>320</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F32" s="3" t="n">
         <v>6</v>
@@ -1141,7 +1141,7 @@
         <v>390</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="F33" s="3" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
Reorder test types in visualizer. Regenerate
</commit_message>
<xml_diff>
--- a/experiment_results/manual_vs_auto.xlsx
+++ b/experiment_results/manual_vs_auto.xlsx
@@ -646,7 +646,7 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>GROUP BY + AGGREGATE</t>
+          <t>AGGREGATION</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -898,7 +898,7 @@
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>LARGE COMPLEX</t>
+          <t>LARGE</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -982,12 +982,12 @@
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>COUNT(*) ROWS</t>
+          <t>COUNT(*)</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>manual_test_one_cell_3</t>
+          <t>manual_test_agg_all_3</t>
         </is>
       </c>
       <c r="C26" s="3" t="n">
@@ -1007,7 +1007,7 @@
       <c r="A27" s="3" t="n"/>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>auto_test_one_cell_3</t>
+          <t>auto_test_agg_all_3</t>
         </is>
       </c>
       <c r="C27" s="3" t="n">
@@ -1027,7 +1027,7 @@
       <c r="A28" s="3" t="n"/>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>manual_test_one_cell_5</t>
+          <t>manual_test_agg_all_5</t>
         </is>
       </c>
       <c r="C28" s="3" t="n">
@@ -1047,7 +1047,7 @@
       <c r="A29" s="3" t="n"/>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>auto_test_one_cell_5</t>
+          <t>auto_test_agg_all_5</t>
         </is>
       </c>
       <c r="C29" s="3" t="n">

</xml_diff>